<commit_message>
changed transition: day/night for each layer
excel file contains easy way for editing and pasting code
fixed night sky colour
</commit_message>
<xml_diff>
--- a/sunPositions.xlsx
+++ b/sunPositions.xlsx
@@ -24,9 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>daySkyFade</t>
+    <t>foregroundFadeAmount</t>
+  </si>
+  <si>
+    <t>midgroundFadeAmount</t>
+  </si>
+  <si>
+    <t>backgroundFadeAmount</t>
+  </si>
+  <si>
+    <t>skyDayFadeAmount</t>
   </si>
 </sst>
 </file>
@@ -50,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -62,15 +71,11 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -79,9 +84,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -92,8 +95,24 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -101,13 +120,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,200 +409,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AB4"/>
+  <dimension ref="B1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="4.140625" customWidth="1"/>
-    <col min="27" max="27" width="2.42578125" customWidth="1"/>
-    <col min="28" max="28" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="27" width="4.140625" customWidth="1"/>
+    <col min="28" max="28" width="96.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:28" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>4</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>5</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>6</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>7</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <v>8</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="3">
         <v>9</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="3">
         <v>10</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="3">
         <v>11</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="3">
         <v>12</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="3">
         <v>13</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2" s="3">
         <v>14</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="3">
         <v>15</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="3">
         <v>16</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T2" s="3">
         <v>17</v>
       </c>
-      <c r="U2" s="1">
+      <c r="U2" s="3">
         <v>18</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="3">
         <v>19</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2" s="3">
         <v>20</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X2" s="3">
         <v>21</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Y2" s="3">
         <v>22</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="Z2" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
         <v>0.2</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="6">
         <v>0.4</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="6">
         <v>0.6</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="6">
         <v>0.8</v>
       </c>
-      <c r="K3" s="3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3">
-        <v>1</v>
-      </c>
-      <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="3">
-        <v>1</v>
-      </c>
-      <c r="P3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>1</v>
-      </c>
-      <c r="R3" s="3">
-        <v>1</v>
-      </c>
-      <c r="S3" s="3">
-        <v>1</v>
-      </c>
-      <c r="T3" s="3">
+      <c r="K3" s="6">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>1</v>
+      </c>
+      <c r="R3" s="6">
+        <v>1</v>
+      </c>
+      <c r="S3" s="6">
+        <v>1</v>
+      </c>
+      <c r="T3" s="6">
+        <v>1</v>
+      </c>
+      <c r="U3" s="5">
         <v>0.8</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="5">
         <v>0.6</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="5">
         <v>0.4</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="5">
         <v>0.2</v>
       </c>
-      <c r="X3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="4">
+      <c r="Y3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5">
         <v>0</v>
       </c>
       <c r="AB3" t="str">
-        <f>CONCATENATE("[",C3,", ",D3,", ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,", ",K3,", ",L3,", ",M3,", ",N3,", ",O3,", ",P3,", ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", ",V3,", ",W3,", ",X3,", ",Y3,", ",Z3,"];")</f>
-        <v>[0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.8, 0.6, 0.4, 0.2, 0, 0, 0];</v>
+        <f>CONCATENATE("var ",B3, " = [",C3,", ",D3,", ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,", ",K3,", ",L3,", ",M3,", ",N3,", ",O3,", ",P3,", ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", ",V3,", ",W3,", ",X3,", ",Y3,", ",Z3,"];")</f>
+        <v>var skyDayFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.8, 0.6, 0.4, 0.2, 0, 0];</v>
       </c>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="Z4" s="1"/>
+    <row r="4" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="W4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="X4" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" ref="AB4:AB6" si="0">CONCATENATE("var ",B4, " = [",C4,", ",D4,", ",E4,", ",F4,", ",G4,", ",H4,", ",I4,", ",J4,", ",K4,", ",L4,", ",M4,", ",N4,", ",O4,", ",P4,", ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", ",V4,", ",W4,", ",X4,", ",Y4,", ",Z4,"];")</f>
+        <v>var backgroundFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 2, 0, 0];</v>
+      </c>
     </row>
+    <row r="5" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="V5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="W5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="str">
+        <f t="shared" si="0"/>
+        <v>var midgroundFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0];</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <v>1</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1</v>
+      </c>
+      <c r="P6" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7">
+        <v>1</v>
+      </c>
+      <c r="S6" s="7">
+        <v>1</v>
+      </c>
+      <c r="T6" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="U6" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="V6" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="W6" s="7">
+        <v>0</v>
+      </c>
+      <c r="X6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" si="0"/>
+        <v>var foregroundFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0, 0];</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added moving stars (needs better art and movement)
</commit_message>
<xml_diff>
--- a/sunPositions.xlsx
+++ b/sunPositions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>foregroundFadeAmount</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>skyDayFadeAmount</t>
+  </si>
+  <si>
+    <t>starsCoorX</t>
+  </si>
+  <si>
+    <t>starsCoorY</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AB7"/>
+  <dimension ref="B1:AB12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,23 +515,23 @@
       <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>0</v>
       </c>
       <c r="F3" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G3" s="6">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H3" s="6">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="I3" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J3" s="6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K3" s="6">
         <v>1</v>
@@ -577,11 +583,11 @@
       </c>
       <c r="AB3" t="str">
         <f>CONCATENATE("var ",B3, " = [",C3,", ",D3,", ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,", ",K3,", ",L3,", ",M3,", ",N3,", ",O3,", ",P3,", ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", ",V3,", ",W3,", ",X3,", ",Y3,", ",Z3,"];")</f>
-        <v>var skyDayFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.8, 0.6, 0.4, 0.2, 0, 0];</v>
+        <v>var skyDayFadeAmount = [0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.8, 0.6, 0.4, 0.2, 0, 0];</v>
       </c>
     </row>
-    <row r="4" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1">
@@ -594,61 +600,61 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="X4" s="1">
         <v>0.2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1">
-        <v>1</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1">
-        <v>1</v>
-      </c>
-      <c r="U4" s="1">
-        <v>1</v>
-      </c>
-      <c r="V4" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="W4" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="X4" s="7">
-        <v>2</v>
       </c>
       <c r="Y4" s="1">
         <v>0</v>
@@ -658,10 +664,10 @@
       </c>
       <c r="AB4" t="str">
         <f t="shared" ref="AB4:AB6" si="0">CONCATENATE("var ",B4, " = [",C4,", ",D4,", ",E4,", ",F4,", ",G4,", ",H4,", ",I4,", ",J4,", ",K4,", ",L4,", ",M4,", ",N4,", ",O4,", ",P4,", ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", ",V4,", ",W4,", ",X4,", ",Y4,", ",Z4,"];")</f>
-        <v>var backgroundFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 2, 0, 0];</v>
+        <v>var backgroundFadeAmount = [0, 0, 0, 0.1, 0.3, 0.5, 0.7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.2, 0, 0];</v>
       </c>
     </row>
-    <row r="5" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -678,16 +684,16 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H5" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="I5" s="1">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="1">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -719,13 +725,13 @@
       <c r="T5" s="1">
         <v>1</v>
       </c>
-      <c r="U5" s="7">
+      <c r="U5" s="1">
         <v>0.7</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="1">
         <v>0.5</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="1">
         <v>0.3</v>
       </c>
       <c r="X5" s="1">
@@ -739,11 +745,11 @@
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="0"/>
-        <v>var midgroundFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0];</v>
+        <v>var midgroundFadeAmount = [0, 0, 0, 0, 0.1, 0.3, 0.5, 0.7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0];</v>
       </c>
     </row>
-    <row r="6" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="7">
@@ -759,19 +765,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="7">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I6" s="7">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="J6" s="7">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="K6" s="7">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="L6" s="7">
         <v>1</v>
@@ -820,10 +826,248 @@
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="0"/>
-        <v>var foregroundFadeAmount = [0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0, 0];</v>
+        <v>var foregroundFadeAmount = [0, 0, 0, 0, 0, 0.1, 0.3, 0.5, 0.7, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0, 0];</v>
       </c>
     </row>
     <row r="7" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3">
+        <v>7</v>
+      </c>
+      <c r="K9" s="3">
+        <v>8</v>
+      </c>
+      <c r="L9" s="3">
+        <v>9</v>
+      </c>
+      <c r="M9" s="3">
+        <v>10</v>
+      </c>
+      <c r="N9" s="3">
+        <v>11</v>
+      </c>
+      <c r="O9" s="3">
+        <v>12</v>
+      </c>
+      <c r="P9" s="3">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>14</v>
+      </c>
+      <c r="R9" s="3">
+        <v>15</v>
+      </c>
+      <c r="S9" s="3">
+        <v>16</v>
+      </c>
+      <c r="T9" s="3">
+        <v>17</v>
+      </c>
+      <c r="U9" s="3">
+        <v>18</v>
+      </c>
+      <c r="V9" s="3">
+        <v>19</v>
+      </c>
+      <c r="W9" s="3">
+        <v>20</v>
+      </c>
+      <c r="X9" s="3">
+        <v>21</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>22</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5">
+        <v>45</v>
+      </c>
+      <c r="F10" s="5">
+        <v>50</v>
+      </c>
+      <c r="G10" s="5">
+        <v>55</v>
+      </c>
+      <c r="H10" s="5">
+        <v>60</v>
+      </c>
+      <c r="I10" s="5">
+        <v>65</v>
+      </c>
+      <c r="J10" s="5">
+        <v>70</v>
+      </c>
+      <c r="K10" s="5">
+        <v>75</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0</v>
+      </c>
+      <c r="U10" s="5">
+        <v>5</v>
+      </c>
+      <c r="V10" s="5">
+        <v>10</v>
+      </c>
+      <c r="W10" s="5">
+        <v>15</v>
+      </c>
+      <c r="X10" s="5">
+        <v>20</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>25</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>30</v>
+      </c>
+      <c r="AB10" t="str">
+        <f>CONCATENATE("var ",B10, " = [",C10,", ",D10,", ",E10,", ",F10,", ",G10,", ",H10,", ",I10,", ",J10,", ",K10,", ",L10,", ",M10,", ",N10,", ",O10,", ",P10,", ",Q10,", ",R10,", ",S10,", ",T10,", ",U10,", ",V10,", ",W10,", ",X10,", ",Y10,", ",Z10,"];")</f>
+        <v>var starsCoorX = [35, 40, 45, 50, 55, 60, 65, 70, 75, 0, 0, 0, 0, 0, 0, 0, 0, 0, 5, 10, 15, 20, 25, 30];</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>0</v>
+      </c>
+      <c r="R11" s="7">
+        <v>0</v>
+      </c>
+      <c r="S11" s="7">
+        <v>0</v>
+      </c>
+      <c r="T11" s="7">
+        <v>0</v>
+      </c>
+      <c r="U11" s="7">
+        <v>0</v>
+      </c>
+      <c r="V11" s="7">
+        <v>0</v>
+      </c>
+      <c r="W11" s="7">
+        <v>0</v>
+      </c>
+      <c r="X11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" ref="AB11" si="1">CONCATENATE("var ",B11, " = [",C11,", ",D11,", ",E11,", ",F11,", ",G11,", ",H11,", ",I11,", ",J11,", ",K11,", ",L11,", ",M11,", ",N11,", ",O11,", ",P11,", ",Q11,", ",R11,", ",S11,", ",T11,", ",U11,", ",V11,", ",W11,", ",X11,", ",Y11,", ",Z11,"];")</f>
+        <v>var starsCoorY = [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0];</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
gradient dawn and dusk added
</commit_message>
<xml_diff>
--- a/sunPositions.xlsx
+++ b/sunPositions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>foregroundFadeAmount</t>
   </si>
@@ -35,13 +35,19 @@
     <t>backgroundFadeAmount</t>
   </si>
   <si>
-    <t>skyDayFadeAmount</t>
-  </si>
-  <si>
     <t>starsCoorX</t>
   </si>
   <si>
     <t>starsCoorY</t>
+  </si>
+  <si>
+    <t>dawnFadeAmount</t>
+  </si>
+  <si>
+    <t>nightSkyFadeAmount</t>
+  </si>
+  <si>
+    <t>duskFadeAmount</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AB12"/>
+  <dimension ref="B1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,88 +513,88 @@
     </row>
     <row r="3" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0</v>
+      </c>
+      <c r="T3" s="6">
+        <v>0</v>
+      </c>
+      <c r="U3" s="6">
         <v>0.2</v>
       </c>
-      <c r="G3" s="6">
+      <c r="V3" s="6">
         <v>0.4</v>
       </c>
-      <c r="H3" s="6">
+      <c r="W3" s="6">
         <v>0.6</v>
       </c>
-      <c r="I3" s="6">
+      <c r="X3" s="6">
         <v>0.8</v>
       </c>
-      <c r="J3" s="6">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6">
-        <v>1</v>
-      </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3" s="6">
-        <v>1</v>
-      </c>
-      <c r="N3" s="6">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6">
-        <v>1</v>
-      </c>
-      <c r="P3" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>1</v>
-      </c>
-      <c r="R3" s="6">
-        <v>1</v>
-      </c>
-      <c r="S3" s="6">
-        <v>1</v>
-      </c>
-      <c r="T3" s="6">
-        <v>1</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="V3" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="W3" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="X3" s="5">
-        <v>0.2</v>
-      </c>
       <c r="Y3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3" t="str">
         <f>CONCATENATE("var ",B3, " = [",C3,", ",D3,", ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,", ",K3,", ",L3,", ",M3,", ",N3,", ",O3,", ",P3,", ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", ",V3,", ",W3,", ",X3,", ",Y3,", ",Z3,"];")</f>
-        <v>var skyDayFadeAmount = [0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.8, 0.6, 0.4, 0.2, 0, 0];</v>
+        <v>var nightSkyFadeAmount = [1, 1, 1, 0.8, 0.6, 0.4, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0.2, 0.4, 0.6, 0.8, 1, 1];</v>
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -600,13 +606,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I4" s="1">
         <v>0.7</v>
@@ -615,46 +621,46 @@
         <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="L4" s="1">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="M4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="W4" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X4" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="1">
         <v>0</v>
@@ -663,13 +669,13 @@
         <v>0</v>
       </c>
       <c r="AB4" t="str">
-        <f t="shared" ref="AB4:AB6" si="0">CONCATENATE("var ",B4, " = [",C4,", ",D4,", ",E4,", ",F4,", ",G4,", ",H4,", ",I4,", ",J4,", ",K4,", ",L4,", ",M4,", ",N4,", ",O4,", ",P4,", ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", ",V4,", ",W4,", ",X4,", ",Y4,", ",Z4,"];")</f>
-        <v>var backgroundFadeAmount = [0, 0, 0, 0.1, 0.3, 0.5, 0.7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.2, 0, 0];</v>
+        <f>CONCATENATE("var ",B4, " = [",C4,", ",D4,", ",E4,", ",F4,", ",G4,", ",H4,", ",I4,", ",J4,", ",K4,", ",L4,", ",M4,", ",N4,", ",O4,", ",P4,", ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", ",V4,", ",W4,", ",X4,", ",Y4,", ",Z4,"];")</f>
+        <v>var dawnFadeAmount = [0, 0, 0, 0, 0, 0.4, 0.7, 1, 0.7, 0.4, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0];</v>
       </c>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -684,390 +690,552 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="str">
+        <f>CONCATENATE("var ",B5, " = [",C5,", ",D5,", ",E5,", ",F5,", ",G5,", ",H5,", ",I5,", ",J5,", ",K5,", ",L5,", ",M5,", ",N5,", ",O5,", ",P5,", ",Q5,", ",R5,", ",S5,", ",T5,", ",U5,", ",V5,", ",W5,", ",X5,", ",Y5,", ",Z5,"];")</f>
+        <v>var duskFadeAmount = [0, 0, 0, 0, 0, 0.4, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0.4, 0.8, 0.4, 0, 0, 0];</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
         <v>0.1</v>
       </c>
-      <c r="H5" s="1">
+      <c r="G6" s="1">
         <v>0.3</v>
       </c>
-      <c r="I5" s="1">
+      <c r="H6" s="1">
         <v>0.5</v>
       </c>
-      <c r="J5" s="1">
+      <c r="I6" s="1">
         <v>0.7</v>
       </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1</v>
-      </c>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1">
-        <v>1</v>
-      </c>
-      <c r="U5" s="1">
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1">
         <v>0.7</v>
       </c>
-      <c r="V5" s="1">
+      <c r="W6" s="1">
         <v>0.5</v>
       </c>
-      <c r="W5" s="1">
+      <c r="X6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" ref="AB6" si="0">CONCATENATE("var ",B6, " = [",C6,", ",D6,", ",E6,", ",F6,", ",G6,", ",H6,", ",I6,", ",J6,", ",K6,", ",L6,", ",M6,", ",N6,", ",O6,", ",P6,", ",Q6,", ",R6,", ",S6,", ",T6,", ",U6,", ",V6,", ",W6,", ",X6,", ",Y6,", ",Z6,"];")</f>
+        <v>var backgroundFadeAmount = [0, 0, 0, 0.1, 0.3, 0.5, 0.7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.2, 0, 0];</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.3</v>
       </c>
-      <c r="X5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="str">
-        <f t="shared" si="0"/>
+      <c r="I7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="str">
+        <f t="shared" ref="AB7:AB8" si="1">CONCATENATE("var ",B7, " = [",C7,", ",D7,", ",E7,", ",F7,", ",G7,", ",H7,", ",I7,", ",J7,", ",K7,", ",L7,", ",M7,", ",N7,", ",O7,", ",P7,", ",Q7,", ",R7,", ",S7,", ",T7,", ",U7,", ",V7,", ",W7,", ",X7,", ",Y7,", ",Z7,"];")</f>
         <v>var midgroundFadeAmount = [0, 0, 0, 0, 0.1, 0.3, 0.5, 0.7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0];</v>
       </c>
     </row>
-    <row r="6" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
+    <row r="8" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
         <v>0.1</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I8" s="7">
         <v>0.3</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J8" s="7">
         <v>0.5</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K8" s="7">
         <v>0.7</v>
       </c>
-      <c r="L6" s="7">
-        <v>1</v>
-      </c>
-      <c r="M6" s="7">
-        <v>1</v>
-      </c>
-      <c r="N6" s="7">
-        <v>1</v>
-      </c>
-      <c r="O6" s="7">
-        <v>1</v>
-      </c>
-      <c r="P6" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>1</v>
-      </c>
-      <c r="R6" s="7">
-        <v>1</v>
-      </c>
-      <c r="S6" s="7">
-        <v>1</v>
-      </c>
-      <c r="T6" s="7">
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>1</v>
+      </c>
+      <c r="O8" s="7">
+        <v>1</v>
+      </c>
+      <c r="P8" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7">
+        <v>1</v>
+      </c>
+      <c r="S8" s="7">
+        <v>1</v>
+      </c>
+      <c r="T8" s="7">
         <v>0.7</v>
       </c>
-      <c r="U6" s="7">
+      <c r="U8" s="7">
         <v>0.5</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V8" s="7">
         <v>0.3</v>
       </c>
-      <c r="W6" s="7">
-        <v>0</v>
-      </c>
-      <c r="X6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="str">
-        <f t="shared" si="0"/>
+      <c r="W8" s="7">
+        <v>0</v>
+      </c>
+      <c r="X8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="str">
+        <f t="shared" si="1"/>
         <v>var foregroundFadeAmount = [0, 0, 0, 0, 0, 0.1, 0.3, 0.5, 0.7, 1, 1, 1, 1, 1, 1, 1, 1, 0.7, 0.5, 0.3, 0, 0, 0, 0];</v>
       </c>
     </row>
-    <row r="7" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
+    <row r="9" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
         <v>2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F11" s="3">
         <v>3</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G11" s="3">
         <v>4</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H11" s="3">
         <v>5</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I11" s="3">
         <v>6</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J11" s="3">
         <v>7</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K11" s="3">
         <v>8</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L11" s="3">
         <v>9</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M11" s="3">
         <v>10</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N11" s="3">
         <v>11</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O11" s="3">
         <v>12</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P11" s="3">
         <v>13</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q11" s="3">
         <v>14</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R11" s="3">
         <v>15</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S11" s="3">
         <v>16</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T11" s="3">
         <v>17</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U11" s="3">
         <v>18</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V11" s="3">
         <v>19</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W11" s="3">
         <v>20</v>
       </c>
-      <c r="X9" s="3">
+      <c r="X11" s="3">
         <v>21</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y11" s="3">
         <v>22</v>
       </c>
-      <c r="Z9" s="4">
+      <c r="Z11" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="12" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>35</v>
+      </c>
+      <c r="D12" s="5">
+        <v>40</v>
+      </c>
+      <c r="E12" s="5">
+        <v>45</v>
+      </c>
+      <c r="F12" s="5">
+        <v>50</v>
+      </c>
+      <c r="G12" s="5">
+        <v>55</v>
+      </c>
+      <c r="H12" s="5">
+        <v>60</v>
+      </c>
+      <c r="I12" s="5">
+        <v>65</v>
+      </c>
+      <c r="J12" s="5">
+        <v>70</v>
+      </c>
+      <c r="K12" s="5">
+        <v>75</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>0</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0</v>
+      </c>
+      <c r="S12" s="5">
+        <v>0</v>
+      </c>
+      <c r="T12" s="5">
+        <v>0</v>
+      </c>
+      <c r="U12" s="5">
+        <v>5</v>
+      </c>
+      <c r="V12" s="5">
+        <v>10</v>
+      </c>
+      <c r="W12" s="5">
+        <v>15</v>
+      </c>
+      <c r="X12" s="5">
+        <v>20</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>25</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>30</v>
+      </c>
+      <c r="AB12" t="str">
+        <f>CONCATENATE("var ",B12, " = [",C12,", ",D12,", ",E12,", ",F12,", ",G12,", ",H12,", ",I12,", ",J12,", ",K12,", ",L12,", ",M12,", ",N12,", ",O12,", ",P12,", ",Q12,", ",R12,", ",S12,", ",T12,", ",U12,", ",V12,", ",W12,", ",X12,", ",Y12,", ",Z12,"];")</f>
+        <v>var starsCoorX = [35, 40, 45, 50, 55, 60, 65, 70, 75, 0, 0, 0, 0, 0, 0, 0, 0, 0, 5, 10, 15, 20, 25, 30];</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5">
-        <v>40</v>
-      </c>
-      <c r="E10" s="5">
-        <v>45</v>
-      </c>
-      <c r="F10" s="5">
-        <v>50</v>
-      </c>
-      <c r="G10" s="5">
-        <v>55</v>
-      </c>
-      <c r="H10" s="5">
-        <v>60</v>
-      </c>
-      <c r="I10" s="5">
-        <v>65</v>
-      </c>
-      <c r="J10" s="5">
-        <v>70</v>
-      </c>
-      <c r="K10" s="5">
-        <v>75</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>0</v>
-      </c>
-      <c r="R10" s="5">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5">
-        <v>0</v>
-      </c>
-      <c r="T10" s="5">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5">
-        <v>5</v>
-      </c>
-      <c r="V10" s="5">
-        <v>10</v>
-      </c>
-      <c r="W10" s="5">
-        <v>15</v>
-      </c>
-      <c r="X10" s="5">
-        <v>20</v>
-      </c>
-      <c r="Y10" s="5">
-        <v>25</v>
-      </c>
-      <c r="Z10" s="5">
-        <v>30</v>
-      </c>
-      <c r="AB10" t="str">
-        <f>CONCATENATE("var ",B10, " = [",C10,", ",D10,", ",E10,", ",F10,", ",G10,", ",H10,", ",I10,", ",J10,", ",K10,", ",L10,", ",M10,", ",N10,", ",O10,", ",P10,", ",Q10,", ",R10,", ",S10,", ",T10,", ",U10,", ",V10,", ",W10,", ",X10,", ",Y10,", ",Z10,"];")</f>
-        <v>var starsCoorX = [35, 40, 45, 50, 55, 60, 65, 70, 75, 0, 0, 0, 0, 0, 0, 0, 0, 0, 5, 10, 15, 20, 25, 30];</v>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
+        <v>0</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>0</v>
+      </c>
+      <c r="R13" s="7">
+        <v>0</v>
+      </c>
+      <c r="S13" s="7">
+        <v>0</v>
+      </c>
+      <c r="T13" s="7">
+        <v>0</v>
+      </c>
+      <c r="U13" s="7">
+        <v>0</v>
+      </c>
+      <c r="V13" s="7">
+        <v>0</v>
+      </c>
+      <c r="W13" s="7">
+        <v>0</v>
+      </c>
+      <c r="X13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="str">
+        <f t="shared" ref="AB13" si="2">CONCATENATE("var ",B13, " = [",C13,", ",D13,", ",E13,", ",F13,", ",G13,", ",H13,", ",I13,", ",J13,", ",K13,", ",L13,", ",M13,", ",N13,", ",O13,", ",P13,", ",Q13,", ",R13,", ",S13,", ",T13,", ",U13,", ",V13,", ",W13,", ",X13,", ",Y13,", ",Z13,"];")</f>
+        <v>var starsCoorY = [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0];</v>
       </c>
     </row>
-    <row r="11" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7">
-        <v>0</v>
-      </c>
-      <c r="M11" s="7">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
-        <v>0</v>
-      </c>
-      <c r="P11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>0</v>
-      </c>
-      <c r="R11" s="7">
-        <v>0</v>
-      </c>
-      <c r="S11" s="7">
-        <v>0</v>
-      </c>
-      <c r="T11" s="7">
-        <v>0</v>
-      </c>
-      <c r="U11" s="7">
-        <v>0</v>
-      </c>
-      <c r="V11" s="7">
-        <v>0</v>
-      </c>
-      <c r="W11" s="7">
-        <v>0</v>
-      </c>
-      <c r="X11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="str">
-        <f t="shared" ref="AB11" si="1">CONCATENATE("var ",B11, " = [",C11,", ",D11,", ",E11,", ",F11,", ",G11,", ",H11,", ",I11,", ",J11,", ",K11,", ",L11,", ",M11,", ",N11,", ",O11,", ",P11,", ",Q11,", ",R11,", ",S11,", ",T11,", ",U11,", ",V11,", ",W11,", ",X11,", ",Y11,", ",Z11,"];")</f>
-        <v>var starsCoorY = [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0];</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed sun and moon (hopefully)
</commit_message>
<xml_diff>
--- a/sunPositions.xlsx
+++ b/sunPositions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>foregroundFadeAmount</t>
   </si>
@@ -48,6 +48,24 @@
   </si>
   <si>
     <t>duskFadeAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunCoorX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunCoorY </t>
+  </si>
+  <si>
+    <t>moonCoorX</t>
+  </si>
+  <si>
+    <t>moonCoorY</t>
+  </si>
+  <si>
+    <t>sunFadeAmount</t>
+  </si>
+  <si>
+    <t>moonFadeAmount</t>
   </si>
 </sst>
 </file>
@@ -421,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AB14"/>
+  <dimension ref="B1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,11 +1249,498 @@
         <v>0</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" ref="AB13" si="2">CONCATENATE("var ",B13, " = [",C13,", ",D13,", ",E13,", ",F13,", ",G13,", ",H13,", ",I13,", ",J13,", ",K13,", ",L13,", ",M13,", ",N13,", ",O13,", ",P13,", ",Q13,", ",R13,", ",S13,", ",T13,", ",U13,", ",V13,", ",W13,", ",X13,", ",Y13,", ",Z13,"];")</f>
+        <f t="shared" ref="AB13:AB19" si="2">CONCATENATE("var ",B13, " = [",C13,", ",D13,", ",E13,", ",F13,", ",G13,", ",H13,", ",I13,", ",J13,", ",K13,", ",L13,", ",M13,", ",N13,", ",O13,", ",P13,", ",Q13,", ",R13,", ",S13,", ",T13,", ",U13,", ",V13,", ",W13,", ",X13,", ",Y13,", ",Z13,"];")</f>
         <v>var starsCoorY = [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0];</v>
       </c>
     </row>
-    <row r="14" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>57</v>
+      </c>
+      <c r="H14">
+        <v>57</v>
+      </c>
+      <c r="I14">
+        <v>85</v>
+      </c>
+      <c r="J14">
+        <v>130</v>
+      </c>
+      <c r="K14">
+        <v>185</v>
+      </c>
+      <c r="L14">
+        <v>256</v>
+      </c>
+      <c r="M14">
+        <v>346</v>
+      </c>
+      <c r="N14">
+        <v>448</v>
+      </c>
+      <c r="O14">
+        <v>535</v>
+      </c>
+      <c r="P14">
+        <v>599</v>
+      </c>
+      <c r="Q14">
+        <v>662</v>
+      </c>
+      <c r="R14">
+        <v>727</v>
+      </c>
+      <c r="S14">
+        <v>779</v>
+      </c>
+      <c r="T14">
+        <v>830</v>
+      </c>
+      <c r="U14">
+        <v>872</v>
+      </c>
+      <c r="V14">
+        <v>914</v>
+      </c>
+      <c r="W14">
+        <v>952</v>
+      </c>
+      <c r="X14">
+        <v>984</v>
+      </c>
+      <c r="Y14">
+        <v>984</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="str">
+        <f t="shared" si="2"/>
+        <v>var sunCoorX  = [0, 0, 0, 0, 57, 57, 85, 130, 185, 256, 346, 448, 535, 599, 662, 727, 779, 830, 872, 914, 952, 984, 984, 0];</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>442</v>
+      </c>
+      <c r="H15">
+        <v>442</v>
+      </c>
+      <c r="I15">
+        <v>370</v>
+      </c>
+      <c r="J15">
+        <v>305</v>
+      </c>
+      <c r="K15">
+        <v>229</v>
+      </c>
+      <c r="L15">
+        <v>160</v>
+      </c>
+      <c r="M15">
+        <v>102</v>
+      </c>
+      <c r="N15">
+        <v>65</v>
+      </c>
+      <c r="O15">
+        <v>51</v>
+      </c>
+      <c r="P15">
+        <v>60</v>
+      </c>
+      <c r="Q15">
+        <v>72</v>
+      </c>
+      <c r="R15">
+        <v>97</v>
+      </c>
+      <c r="S15">
+        <v>125</v>
+      </c>
+      <c r="T15">
+        <v>158</v>
+      </c>
+      <c r="U15">
+        <v>197</v>
+      </c>
+      <c r="V15">
+        <v>241</v>
+      </c>
+      <c r="W15">
+        <v>286</v>
+      </c>
+      <c r="X15">
+        <v>341</v>
+      </c>
+      <c r="Y15">
+        <v>341</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="str">
+        <f t="shared" si="2"/>
+        <v>var sunCoorY  = [0, 0, 0, 0, 442, 442, 370, 305, 229, 160, 102, 65, 51, 60, 72, 97, 125, 158, 197, 241, 286, 341, 341, 0];</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5">
+        <v>525</v>
+      </c>
+      <c r="D16" s="5">
+        <v>618</v>
+      </c>
+      <c r="E16" s="5">
+        <v>713</v>
+      </c>
+      <c r="F16" s="5">
+        <v>797</v>
+      </c>
+      <c r="G16" s="5">
+        <v>871</v>
+      </c>
+      <c r="H16" s="5">
+        <v>932</v>
+      </c>
+      <c r="I16" s="5">
+        <v>999</v>
+      </c>
+      <c r="J16" s="5">
+        <v>999</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>0</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0</v>
+      </c>
+      <c r="S16" s="5">
+        <v>0</v>
+      </c>
+      <c r="T16" s="5">
+        <v>39</v>
+      </c>
+      <c r="U16" s="5">
+        <v>39</v>
+      </c>
+      <c r="V16" s="5">
+        <v>92</v>
+      </c>
+      <c r="W16" s="5">
+        <v>158</v>
+      </c>
+      <c r="X16" s="5">
+        <v>238</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>328</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>434</v>
+      </c>
+      <c r="AB16" t="str">
+        <f t="shared" si="2"/>
+        <v>var moonCoorX = [525, 618, 713, 797, 871, 932, 999, 999, 0, 0, 0, 0, 0, 0, 0, 0, 0, 39, 39, 92, 158, 238, 328, 434];</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="7">
+        <v>36</v>
+      </c>
+      <c r="D17" s="7">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7">
+        <v>83</v>
+      </c>
+      <c r="F17" s="7">
+        <v>130</v>
+      </c>
+      <c r="G17" s="7">
+        <v>198</v>
+      </c>
+      <c r="H17" s="7">
+        <v>271</v>
+      </c>
+      <c r="I17" s="7">
+        <v>403</v>
+      </c>
+      <c r="J17" s="7">
+        <v>403</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+      <c r="O17" s="7">
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>0</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0</v>
+      </c>
+      <c r="S17" s="7">
+        <v>0</v>
+      </c>
+      <c r="T17" s="7">
+        <v>420</v>
+      </c>
+      <c r="U17" s="7">
+        <v>420</v>
+      </c>
+      <c r="V17" s="7">
+        <v>309</v>
+      </c>
+      <c r="W17" s="7">
+        <v>219</v>
+      </c>
+      <c r="X17" s="7">
+        <v>143</v>
+      </c>
+      <c r="Y17" s="7">
+        <v>85</v>
+      </c>
+      <c r="Z17" s="7">
+        <v>49</v>
+      </c>
+      <c r="AB17" t="str">
+        <f t="shared" si="2"/>
+        <v>var moonCoorY = [36, 49, 83, 130, 198, 271, 403, 403, 0, 0, 0, 0, 0, 0, 0, 0, 0, 420, 420, 309, 219, 143, 85, 49];</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1</v>
+      </c>
+      <c r="J19" s="5">
+        <v>1</v>
+      </c>
+      <c r="K19" s="5">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5">
+        <v>1</v>
+      </c>
+      <c r="N19" s="5">
+        <v>1</v>
+      </c>
+      <c r="O19" s="5">
+        <v>1</v>
+      </c>
+      <c r="P19" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>1</v>
+      </c>
+      <c r="R19" s="5">
+        <v>1</v>
+      </c>
+      <c r="S19" s="5">
+        <v>1</v>
+      </c>
+      <c r="T19" s="5">
+        <v>1</v>
+      </c>
+      <c r="U19" s="5">
+        <v>1</v>
+      </c>
+      <c r="V19" s="5">
+        <v>1</v>
+      </c>
+      <c r="W19" s="5">
+        <v>1</v>
+      </c>
+      <c r="X19" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="str">
+        <f t="shared" si="2"/>
+        <v>var sunFadeAmount = [0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0];</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="7">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7">
+        <v>0</v>
+      </c>
+      <c r="P20" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>0</v>
+      </c>
+      <c r="R20" s="7">
+        <v>0</v>
+      </c>
+      <c r="S20" s="7">
+        <v>0</v>
+      </c>
+      <c r="T20" s="7">
+        <v>0</v>
+      </c>
+      <c r="U20" s="7">
+        <v>1</v>
+      </c>
+      <c r="V20" s="7">
+        <v>1</v>
+      </c>
+      <c r="W20" s="7">
+        <v>1</v>
+      </c>
+      <c r="X20" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB20" t="str">
+        <f t="shared" ref="AB20" si="3">CONCATENATE("var ",B20, " = [",C20,", ",D20,", ",E20,", ",F20,", ",G20,", ",H20,", ",I20,", ",J20,", ",K20,", ",L20,", ",M20,", ",N20,", ",O20,", ",P20,", ",Q20,", ",R20,", ",S20,", ",T20,", ",U20,", ",V20,", ",W20,", ",X20,", ",Y20,", ",Z20,"];")</f>
+        <v>var moonFadeAmount = [1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1];</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
all animations and fades execute simultaneously
</commit_message>
<xml_diff>
--- a/sunPositions.xlsx
+++ b/sunPositions.xlsx
@@ -81,12 +81,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -150,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -159,6 +165,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -769,7 +778,7 @@
       </c>
       <c r="AB5" t="str">
         <f>CONCATENATE("var ",B5, " = [",C5,", ",D5,", ",E5,", ",F5,", ",G5,", ",H5,", ",I5,", ",J5,", ",K5,", ",L5,", ",M5,", ",N5,", ",O5,", ",P5,", ",Q5,", ",R5,", ",S5,", ",T5,", ",U5,", ",V5,", ",W5,", ",X5,", ",Y5,", ",Z5,"];")</f>
-        <v>var duskFadeAmount = [0, 0, 0, 0, 0, 0.4, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0.4, 0.8, 0.4, 0, 0, 0];</v>
+        <v>var duskFadeAmount = [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0.4, 0.8, 0.4, 0, 0, 0];</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
@@ -1266,10 +1275,10 @@
       <c r="E14" s="5">
         <v>0</v>
       </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="8">
+        <v>57</v>
+      </c>
+      <c r="G14" s="8">
         <v>57</v>
       </c>
       <c r="H14">
@@ -1323,15 +1332,15 @@
       <c r="X14">
         <v>984</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="8">
         <v>984</v>
       </c>
-      <c r="Z14">
-        <v>0</v>
+      <c r="Z14" s="8">
+        <v>984</v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="2"/>
-        <v>var sunCoorX  = [0, 0, 0, 0, 57, 57, 85, 130, 185, 256, 346, 448, 535, 599, 662, 727, 779, 830, 872, 914, 952, 984, 984, 0];</v>
+        <v>var sunCoorX  = [0, 0, 0, 57, 57, 57, 85, 130, 185, 256, 346, 448, 535, 599, 662, 727, 779, 830, 872, 914, 952, 984, 984, 984];</v>
       </c>
     </row>
     <row r="15" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1347,10 +1356,10 @@
       <c r="E15" s="7">
         <v>0</v>
       </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="8">
+        <v>442</v>
+      </c>
+      <c r="G15" s="8">
         <v>442</v>
       </c>
       <c r="H15">
@@ -1404,15 +1413,15 @@
       <c r="X15">
         <v>341</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="8">
         <v>341</v>
       </c>
-      <c r="Z15">
-        <v>0</v>
+      <c r="Z15" s="8">
+        <v>341</v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="2"/>
-        <v>var sunCoorY  = [0, 0, 0, 0, 442, 442, 370, 305, 229, 160, 102, 65, 51, 60, 72, 97, 125, 158, 197, 241, 286, 341, 341, 0];</v>
+        <v>var sunCoorY  = [0, 0, 0, 442, 442, 442, 370, 305, 229, 160, 102, 65, 51, 60, 72, 97, 125, 158, 197, 241, 286, 341, 341, 341];</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1440,11 +1449,11 @@
       <c r="I16" s="5">
         <v>999</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="9">
         <v>999</v>
       </c>
-      <c r="K16" s="5">
-        <v>0</v>
+      <c r="K16" s="9">
+        <v>999</v>
       </c>
       <c r="L16" s="5">
         <v>0</v>
@@ -1467,10 +1476,10 @@
       <c r="R16" s="5">
         <v>0</v>
       </c>
-      <c r="S16" s="5">
-        <v>0</v>
-      </c>
-      <c r="T16" s="5">
+      <c r="S16" s="9">
+        <v>39</v>
+      </c>
+      <c r="T16" s="9">
         <v>39</v>
       </c>
       <c r="U16" s="5">
@@ -1493,7 +1502,7 @@
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="2"/>
-        <v>var moonCoorX = [525, 618, 713, 797, 871, 932, 999, 999, 0, 0, 0, 0, 0, 0, 0, 0, 0, 39, 39, 92, 158, 238, 328, 434];</v>
+        <v>var moonCoorX = [525, 618, 713, 797, 871, 932, 999, 999, 999, 0, 0, 0, 0, 0, 0, 0, 39, 39, 39, 92, 158, 238, 328, 434];</v>
       </c>
     </row>
     <row r="17" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1521,11 +1530,11 @@
       <c r="I17" s="7">
         <v>403</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="10">
         <v>403</v>
       </c>
-      <c r="K17" s="7">
-        <v>0</v>
+      <c r="K17" s="10">
+        <v>403</v>
       </c>
       <c r="L17" s="7">
         <v>0</v>
@@ -1548,10 +1557,10 @@
       <c r="R17" s="7">
         <v>0</v>
       </c>
-      <c r="S17" s="7">
-        <v>0</v>
-      </c>
-      <c r="T17" s="7">
+      <c r="S17" s="10">
+        <v>420</v>
+      </c>
+      <c r="T17" s="10">
         <v>420</v>
       </c>
       <c r="U17" s="7">
@@ -1574,7 +1583,7 @@
       </c>
       <c r="AB17" t="str">
         <f t="shared" si="2"/>
-        <v>var moonCoorY = [36, 49, 83, 130, 198, 271, 403, 403, 0, 0, 0, 0, 0, 0, 0, 0, 0, 420, 420, 309, 219, 143, 85, 49];</v>
+        <v>var moonCoorY = [36, 49, 83, 130, 198, 271, 403, 403, 403, 0, 0, 0, 0, 0, 0, 0, 420, 420, 420, 309, 219, 143, 85, 49];</v>
       </c>
     </row>
     <row r="18" spans="2:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1646,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="X19" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="5">
         <v>0</v>
@@ -1656,7 +1665,7 @@
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="2"/>
-        <v>var sunFadeAmount = [0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0];</v>
+        <v>var sunFadeAmount = [0, 0, 0, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0];</v>
       </c>
     </row>
     <row r="20" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>